<commit_message>
MS-SITESS update RS code and configure script
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-SITESS/MS-SITESS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-SITESS/MS-SITESS_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10216"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97AC1B-9A06-C540-8D70-6953BB341231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C1110D-457A-B14E-B14A-4F7D4377D71F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16320" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-340" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -4485,10 +4485,6 @@
   </si>
   <si>
     <t>[In CreateWeb] [presence:] If set to false, the online presence information MUST NOT be enabled for the subsite to be created. &lt;17&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix B: Product Behavior] Implementation does be enabled for the subsite to be created, when presence set to omitted, and anonymous authentication is not allowed for the subsite.  &lt;17&gt; Section 3.1.4.9.2.1:  If anonymous authentication is not allowed for the subsite, the online presence information will be enabled on SharePoint Foundation 2010.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -4592,6 +4588,10 @@
   </si>
   <si>
     <t>5.3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does be enabled for the subsite to be created, when presence set to omitted, and anonymous authentication is not allowed for the subsite.  &lt;17&gt; Section 3.1.4.9.2.1:  If anonymous authentication is not allowed for the subsite, the online presence information will be enabled on SharePoint Foundation 2010 and Microsoft SharePoint Foundation 2013 Service Pack 1 (SP1).</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5101,6 +5101,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5163,27 +5184,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16589,13 +16589,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M529"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A517" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C521" sqref="C521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="78" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
@@ -16644,7 +16644,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>993</v>
@@ -16658,49 +16658,49 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="19">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="109"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="88"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="112"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="91"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="92" t="s">
         <v>908</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
       <c r="J6" s="47"/>
       <c r="K6" s="2"/>
     </row>
@@ -16708,32 +16708,32 @@
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="114" t="s">
+      <c r="B7" s="93" t="s">
         <v>909</v>
       </c>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="15">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
       <c r="J8" s="47"/>
       <c r="K8" s="2"/>
     </row>
@@ -16741,16 +16741,16 @@
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="100" t="s">
         <v>915</v>
       </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="95"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
       <c r="J9" s="47"/>
       <c r="K9" s="2"/>
     </row>
@@ -16758,16 +16758,16 @@
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="103" t="s">
         <v>916</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="98"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="105"/>
       <c r="J10" s="47"/>
       <c r="K10" s="2"/>
     </row>
@@ -16775,16 +16775,16 @@
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="99" t="s">
         <v>910</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
@@ -16797,12 +16797,12 @@
       <c r="C12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="101"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="108"/>
       <c r="J12" s="47"/>
       <c r="K12" s="2"/>
     </row>
@@ -16816,12 +16816,12 @@
       <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="104"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="111"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15">
@@ -16834,12 +16834,12 @@
       <c r="C14" s="9" t="s">
         <v>912</v>
       </c>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="104"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="111"/>
       <c r="J14" s="47"/>
       <c r="K14" s="2"/>
     </row>
@@ -16853,28 +16853,28 @@
       <c r="C15" s="9" t="s">
         <v>913</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="107"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="114"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="94" t="s">
         <v>917</v>
       </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
       <c r="J16" s="47"/>
       <c r="K16" s="2"/>
     </row>
@@ -16882,32 +16882,32 @@
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="89" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="91"/>
+      <c r="B17" s="96" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="98"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="30" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="99" t="s">
         <v>914</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
       <c r="J18" s="47"/>
       <c r="K18" s="2"/>
       <c r="M18" s="2"/>
@@ -28959,7 +28959,7 @@
         <v>845</v>
       </c>
       <c r="C495" s="13" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D495" s="53" t="s">
         <v>945</v>
@@ -29621,7 +29621,7 @@
         <v>845</v>
       </c>
       <c r="C519" s="13" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D519" s="7" t="s">
         <v>1108</v>
@@ -29650,7 +29650,7 @@
         <v>845</v>
       </c>
       <c r="C520" s="13" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D520" s="7" t="s">
         <v>1108</v>
@@ -29671,7 +29671,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="521" spans="1:10" ht="76" thickBot="1">
+    <row r="521" spans="1:10" ht="91" thickBot="1">
       <c r="A521" s="7" t="s">
         <v>1124</v>
       </c>
@@ -29679,7 +29679,7 @@
         <v>845</v>
       </c>
       <c r="C521" s="13" t="s">
-        <v>1215</v>
+        <v>1221</v>
       </c>
       <c r="D521" s="53" t="s">
         <v>1110</v>
@@ -29708,7 +29708,7 @@
         <v>845</v>
       </c>
       <c r="C522" s="13" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D522" s="53" t="s">
         <v>1110</v>
@@ -29923,11 +29923,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
@@ -29935,6 +29930,11 @@
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G406:G417 F415:F416 F374:F375 F330:F331 G318:G331 F297:F298 G294:G298 F279:F280 G271:G280 F213:F214 G194:G216 G186:G190 G156:G160 G111:G116 G23:G80 E316:G316 B137:B301 C20:G20 A480:E480 C486:E486 C481:E484 D485:E485 E23:E135 F28:F130 B23:B122 E317:E357 B305:B357 F348:G357 B486:B491 G487:G491 E487:E491 E137:E301 B495:B498 E495:E507 F495:F500 E402:E450 B402:B450 B359:B360 E359:G360 E362:E385 B362:B385 F362:F363 G362:G376">
@@ -37523,21 +37523,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -37586,10 +37571,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37609,16 +37616,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated version for MS-SITESS.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-SITESS/MS-SITESS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-SITESS/MS-SITESS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBF4444-B878-42AE-8A36-AEF57C858085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDE1C39-9683-416A-B960-100CE81B550A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21450" yWindow="3075" windowWidth="21105" windowHeight="12480" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -5094,27 +5094,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5177,6 +5156,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16583,7 +16583,7 @@
   <dimension ref="A1:M529"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -16643,7 +16643,7 @@
         <v>993</v>
       </c>
       <c r="F3" s="56">
-        <v>44397</v>
+        <v>44474</v>
       </c>
       <c r="G3" s="48"/>
       <c r="H3" s="2"/>
@@ -16651,49 +16651,49 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="20.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="88"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="91"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="112"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="113" t="s">
         <v>908</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
       <c r="J6" s="47"/>
       <c r="K6" s="2"/>
     </row>
@@ -16701,32 +16701,32 @@
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="114" t="s">
         <v>909</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
       <c r="J8" s="47"/>
       <c r="K8" s="2"/>
     </row>
@@ -16734,16 +16734,16 @@
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="93" t="s">
         <v>915</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="102"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="95"/>
       <c r="J9" s="47"/>
       <c r="K9" s="2"/>
     </row>
@@ -16751,16 +16751,16 @@
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="96" t="s">
         <v>916</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="105"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="98"/>
       <c r="J10" s="47"/>
       <c r="K10" s="2"/>
     </row>
@@ -16768,16 +16768,16 @@
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="92" t="s">
         <v>910</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
@@ -16790,12 +16790,12 @@
       <c r="C12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="108"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="101"/>
       <c r="J12" s="47"/>
       <c r="K12" s="2"/>
     </row>
@@ -16809,12 +16809,12 @@
       <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="111"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="104"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11">
@@ -16827,12 +16827,12 @@
       <c r="C14" s="9" t="s">
         <v>912</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="111"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="104"/>
       <c r="J14" s="47"/>
       <c r="K14" s="2"/>
     </row>
@@ -16846,28 +16846,28 @@
       <c r="C15" s="9" t="s">
         <v>913</v>
       </c>
-      <c r="D15" s="112"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="114"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
+      <c r="I15" s="107"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="87" t="s">
         <v>917</v>
       </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="88"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="88"/>
       <c r="J16" s="47"/>
       <c r="K16" s="2"/>
     </row>
@@ -16875,32 +16875,32 @@
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="89" t="s">
         <v>1211</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="98"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="91"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="30" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="99" t="s">
+      <c r="B18" s="92" t="s">
         <v>914</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
       <c r="J18" s="47"/>
       <c r="K18" s="2"/>
       <c r="M18" s="2"/>
@@ -29916,6 +29916,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
@@ -29923,11 +29928,6 @@
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G406:G417 F415:F416 F374:F375 F330:F331 G318:G331 F297:F298 G294:G298 F279:F280 G271:G280 F213:F214 G194:G216 G186:G190 G156:G160 G111:G116 G23:G80 E316:G316 B137:B301 C20:G20 A480:E480 C486:E486 C481:E484 D485:E485 E23:E135 F28:F130 B23:B122 E317:E357 B305:B357 F348:G357 B486:B491 G487:G491 E487:E491 E137:E301 B495:B498 E495:E507 F495:F500 E402:E450 B402:B450 B359:B360 E359:G360 E362:E385 B362:B385 F362:F363 G362:G376">
@@ -37565,18 +37565,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37595,6 +37595,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37606,12 +37614,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>